<commit_message>
[Featue] Added Arcadyan Q & A
</commit_message>
<xml_diff>
--- a/TopicRecord.xlsx
+++ b/TopicRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiaki\Qsync\Github\InterviewQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DC8D37-D63A-46D1-8B29-3C1016E692DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E4A52B-B923-4A9D-8158-195FE87F1073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{570E4537-033E-4269-90DB-11406DD7D5A2}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Extra" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C, C++'!$B$1:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'C, C++'!$B$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Company</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -188,6 +188,22 @@
   </si>
   <si>
     <t>DFS</t>
+  </si>
+  <si>
+    <t>Arcadyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logic operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable types</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefix/postfix adder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -560,20 +576,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD58BB5C-6AC7-4082-B706-D5CDC07F67A5}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="23.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -581,138 +598,219 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>SUM(C2)/COUNTA(C2)*100%</f>
+        <f>SUM(C2:D2)/COUNTA(C2:D2)*100%</f>
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A12" si="0">SUM(C3)/COUNTA(C3)*100%</f>
-        <v>1</v>
+        <f>SUM(C3:D3)/COUNTA(C3:D3)*100%</f>
+        <v>0.5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>SUM(C4:D4)/COUNTA(C4:D4)*100%</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" ref="A5:A15" si="0">SUM(C5:D5)/COUNTA(C5:D5)*100%</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <v>0</v>
       </c>
     </row>
@@ -766,7 +864,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C2:C12</xm:sqref>
+          <xm:sqref>C1:D15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -776,19 +874,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162BFA37-839C-49B8-AD90-B90B61D0FCE8}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -796,12 +895,15 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>SUM(C2)/COUNTA(C2)*100%</f>
+        <f>SUM(C2:D2)/COUNTA(C2:D2)*100%</f>
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -810,10 +912,13 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A7" si="0">SUM(C3)/COUNTA(C3)*100%</f>
+        <f t="shared" ref="A3:A7" si="0">SUM(C3:D3)/COUNTA(C3:D3)*100%</f>
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -822,8 +927,11 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -834,20 +942,26 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -858,8 +972,11 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -870,26 +987,34 @@
       <c r="C7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -898,7 +1023,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{5CA5E733-3CBF-4EC0-90D7-CA1A5FED8775}">
+          <x14:cfRule type="iconSet" priority="2" id="{5CA5E733-3CBF-4EC0-90D7-CA1A5FED8775}">
             <x14:iconSet iconSet="5Quarters" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -925,7 +1050,7 @@
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{09CD0E85-9B1C-465A-824B-5F312691BD8D}">
+          <x14:cfRule type="iconSet" priority="3" id="{09CD0E85-9B1C-465A-824B-5F312691BD8D}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -941,7 +1066,26 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C2:C12</xm:sqref>
+          <xm:sqref>C2:D7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{F1169B30-2548-4D69-8510-19AC030926FA}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C1</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -951,19 +1095,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975F82D9-0FF5-4A81-88F9-8C903C4DDDF9}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -971,100 +1116,126 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>SUM(C2)/COUNTA(C2)*100%</f>
-        <v>1</v>
+        <f>SUM(C2:D2)/COUNTA(C2:D2)*100%</f>
+        <v>0.5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A7" si="0">SUM(C3)/COUNTA(C3)*100%</f>
-        <v>1</v>
+        <f t="shared" ref="A3:A7" si="0">SUM(C3:D3)/COUNTA(C3:D3)*100%</f>
+        <v>0.5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1073,7 +1244,331 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{04B3B811-0FDE-4FC5-AFF9-0DAFCAF5C6DB}">
+          <x14:cfRule type="iconSet" priority="3" id="{04B3B811-0FDE-4FC5-AFF9-0DAFCAF5C6DB}">
+            <x14:iconSet iconSet="5Quarters" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="5Quarters" iconId="0"/>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>A1 A8:A1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{FD02F6D6-5D00-482F-8222-B89926F0A703}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C2:D7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{DC848552-4ED8-449D-820D-B26A7741DF0C}">
+            <x14:iconSet iconSet="5Quarters" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="5Quarters" iconId="0"/>
+              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>A2:A7</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24945FDF-70CE-468E-BD87-65E86D7E71B8}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>SUM(C2:D2)/COUNTA(C2:D2)*100%</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A15" si="0">SUM(C3:D3)/COUNTA(C3:D3)*100%</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{D3BBBF2A-BCF4-4A7B-8018-9C9811EFC7E6}">
             <x14:iconSet iconSet="5Quarters" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1100,7 +1595,7 @@
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{FD02F6D6-5D00-482F-8222-B89926F0A703}">
+          <x14:cfRule type="iconSet" priority="3" id="{5318753D-40D0-4DCE-9E09-1411403BE1EA}">
             <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1116,258 +1611,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>C2:C12</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24945FDF-70CE-468E-BD87-65E86D7E71B8}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <f>SUM(C2)/COUNTA(C2)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f>SUM(C3)/COUNTA(C3)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f>SUM(C4)/COUNTA(C4)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f>SUM(C5)/COUNTA(C5)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f>SUM(C6)/COUNTA(C6)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <f t="shared" ref="A7:A15" si="0">SUM(C7)/COUNTA(C7)*100%</f>
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{D3BBBF2A-BCF4-4A7B-8018-9C9811EFC7E6}">
-            <x14:iconSet iconSet="5Quarters" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>20</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>40</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>60</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>80</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="5Quarters" iconId="0"/>
-              <x14:cfIcon iconSet="4RedToBlack" iconId="1"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="1"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>A1:A1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{5318753D-40D0-4DCE-9E09-1411403BE1EA}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>C2:C15</xm:sqref>
+          <xm:sqref>C2:D15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1380,7 +1624,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>